<commit_message>
new MapBox Map added
</commit_message>
<xml_diff>
--- a/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
+++ b/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5_AHIF\SYP(LIN_REL)\TravelAdvisor\SYP(MUH)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Schule\Schuljahr_2019_20\SYP\Github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55225E69-DCA3-4935-B014-1D48A3EB9A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEF3F01-38B4-4B97-9397-5352797A1B42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4488" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productbacklog" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Webservices</t>
   </si>
   <si>
-    <t>Pämien aktivieren/deaktivieren; löschen; filtern</t>
-  </si>
-  <si>
     <t>Webservices definieren</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
   </si>
   <si>
     <t>Iteration 3:</t>
-  </si>
-  <si>
-    <t>Android-App + NoSQL-Usermanagement</t>
   </si>
   <si>
     <t>alle offenen Aufgaben + Userstories umsetzen + Bugfixes ausbessern</t>
@@ -205,12 +199,6 @@
 UserstoryMap erstellen</t>
   </si>
   <si>
-    <t>Locations anzeigen
-Locations erstellen
-Locations bearbeiten
-Locations löschen</t>
-  </si>
-  <si>
     <t>Rezension erstellen</t>
   </si>
   <si>
@@ -221,12 +209,6 @@
   </si>
   <si>
     <t>Rezension anzeigen (Benutzer + Anbieter)</t>
-  </si>
-  <si>
-    <t>Location aktivieren/deaktivieren
-Rezensionen anzeigen
-Rezensionen erstellen
-Rezensionen löschen</t>
   </si>
   <si>
     <t>Location-Detail anzeigen (Benutzer)</t>
@@ -258,6 +240,24 @@
   </si>
   <si>
     <t>Prämien filtern (Benutzer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations anzeigen
+Locations erstellen
+Locations bearbeiten
+</t>
+  </si>
+  <si>
+    <t>Location aktivieren/deaktivieren
+Locations löschen</t>
+  </si>
+  <si>
+    <t>Pämien aktivieren/deaktivieren;
+Prämien löschen
+Prämien filtern</t>
+  </si>
+  <si>
+    <t>Weboberfläche + Android-App + NoSQL-Usermanagement</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,22 +370,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,8 +397,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -419,17 +417,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -656,558 +654,552 @@
   </sheetPr>
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7" t="s">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="7" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A13" s="25" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="5" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="5" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="5" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="5" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="5" t="s">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+      <c r="D26" s="11"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A39" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+    </row>
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="28"/>
+      <c r="C41" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="25"/>
+      <c r="C42" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A39" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-    </row>
-    <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A43" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
+    </row>
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
+    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
+    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
+    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
+    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
+    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
+    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-    </row>
-    <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-    </row>
-    <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
+    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
+    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-    </row>
-    <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
+    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
+    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="13"/>
-    </row>
-    <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-    </row>
-    <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-    </row>
-    <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-    </row>
-    <row r="73" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="11"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-    </row>
-    <row r="74" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
+    <row r="69" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="9"/>
+    </row>
+    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
+    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
       <c r="C75" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A30:B30"/>
@@ -1218,6 +1210,12 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:C3"/>
@@ -1250,108 +1248,108 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="39.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="39.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="33"/>
-    </row>
-    <row r="4" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="33"/>
-    </row>
-    <row r="5" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="25" t="s">
+      <c r="C4" s="31"/>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="34" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="B8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="B9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>64</v>
+      <c r="B10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating map features and styles
</commit_message>
<xml_diff>
--- a/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
+++ b/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Schule\Schuljahr_2019_20\SYP\Github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A696147-0BD1-4E21-BED4-87B5430107C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10056BE-6941-4A14-8C53-6EEA895F2AA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productbacklog" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t xml:space="preserve">*Bemerkung* Obwohl Kleinegger und Gilgenreiner großteils die Weboberfläche mithilfe </t>
   </si>
   <si>
-    <t>der Usertories lösen, kümmert sich Sonnek um das Backend bzw Datenbank verbindung jeder Userstory</t>
-  </si>
-  <si>
     <t>Weboberfläche + Webservice</t>
   </si>
   <si>
@@ -784,6 +781,9 @@
       <t xml:space="preserve">
 Boni-System</t>
     </r>
+  </si>
+  <si>
+    <t>der Usertories lösen, kümmert sich Sonnek um das Backend bzw Datenbankverbindung jeder Userstory</t>
   </si>
 </sst>
 </file>
@@ -964,28 +964,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1212,8 +1212,8 @@
   </sheetPr>
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1225,52 +1225,52 @@
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1283,8 +1283,8 @@
       </c>
       <c r="C7" s="3"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -1301,10 +1301,10 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1324,42 +1324,42 @@
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="33"/>
+      <c r="A13" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="36"/>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" spans="1:10" s="21" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1368,10 +1368,10 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="27"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1380,10 +1380,10 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1392,10 +1392,10 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
@@ -1476,10 +1476,10 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1488,10 +1488,10 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1502,10 +1502,10 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1515,10 +1515,10 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1528,10 +1528,10 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="28"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -1540,10 +1540,10 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="28"/>
+      <c r="A32" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="32"/>
       <c r="C32" s="4" t="s">
         <v>12</v>
       </c>
@@ -1552,10 +1552,10 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="27"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="4" t="s">
         <v>12</v>
       </c>
@@ -1564,10 +1564,10 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="4" t="s">
         <v>12</v>
       </c>
@@ -1576,10 +1576,10 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="27"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1588,10 +1588,10 @@
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="27"/>
+      <c r="A36" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="34"/>
       <c r="C36" s="4" t="s">
         <v>12</v>
       </c>
@@ -1600,10 +1600,10 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="27"/>
+      <c r="A37" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="34"/>
       <c r="C37" s="4" t="s">
         <v>12</v>
       </c>
@@ -1612,20 +1612,20 @@
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
+      <c r="A38" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="32"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1633,10 +1633,10 @@
       <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="32"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="4" t="s">
         <v>7</v>
       </c>
@@ -1644,186 +1644,186 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="33"/>
+      <c r="A42" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="36"/>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="36"/>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="32"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="32"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="32"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="32"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="32"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="32"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="32"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="32"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="31"/>
+      <c r="A53" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="27"/>
       <c r="C53" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="31"/>
+      <c r="A54" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="27"/>
       <c r="C54" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="27"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="33"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="34"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="34"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="4" t="s">
         <v>40</v>
       </c>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1963,13 +1963,34 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="A59:C59"/>
@@ -1986,34 +2007,13 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01238BF-CC45-444D-857F-D850712E7ECB}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="157" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2039,15 +2039,15 @@
       <c r="A1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="38"/>
     </row>
@@ -2056,7 +2056,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="38"/>
     </row>
@@ -2070,11 +2070,11 @@
       <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
@@ -2101,10 +2101,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
@@ -2112,10 +2112,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96.75" x14ac:dyDescent="0.2">
@@ -2123,26 +2123,26 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="11" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2161,10 +2161,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
@@ -2172,10 +2172,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
@@ -2183,10 +2183,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Verwaltungsdokumente für SYP-Projekt
</commit_message>
<xml_diff>
--- a/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
+++ b/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Schule\Schuljahr_2019_20\SYP\Github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10056BE-6941-4A14-8C53-6EEA895F2AA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15664F6E-3F95-410F-AA81-639850FB43A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productbacklog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>Arbeitsaufteilung:</t>
   </si>
@@ -323,6 +323,362 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Beenden der vorgenommen Webservices </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Webapp</t>
+  </si>
+  <si>
+    <t>AndroidApp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prämien anzeigen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location-Detail anzeigen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations anzeigen </t>
+  </si>
+  <si>
+    <t>Firebase - Usermanagement</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prämien erstellen </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Prämien anzeigen (Anbieter) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Prämien bearbeiten x
+UserstoryMap erstellen </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Locations anzeigen AndroidApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Locations-Details anzeigen AndroidApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Locations filtern AndroidApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Location Routenplaner AndroidApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Usermanagement mit Firebase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Login für Webapp mit Firebase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Registrieren für Webapp mit Firebase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <t>der Usertories lösen, kümmert sich Sonnek um das Backend bzw Datenbankverbindung jeder Userstory</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Prämien filtern (Usermanagement) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Boni-System</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pämien aktivieren/deaktivieren </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Prämien löschen </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Prämien bearbeiten </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Userstorymap update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Prämien filtern (Usermanagement) x</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">DB aufsetzen und befüllen </t>
     </r>
     <r>
@@ -367,11 +723,19 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Besitzer/Besucher CRUD x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Besitzer/Besucher CRUD x 
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -433,7 +797,64 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Beenden der vorgenommen Webservices </t>
+      <t xml:space="preserve">Rezensionen anzeigen WebApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rezensionen updaten WebApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rezensionen erstellen WebApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rezensionen löschen WebApp </t>
     </r>
     <r>
       <rPr>
@@ -456,150 +877,29 @@
     </r>
   </si>
   <si>
-    <t>Webapp</t>
-  </si>
-  <si>
-    <t>AndroidApp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prämien anzeigen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location-Detail anzeigen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locations anzeigen </t>
-  </si>
-  <si>
-    <t>Firebase - Usermanagement</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Prämien erstellen </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Prämien anzeigen (Anbieter) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Prämien bearbeiten x
-UserstoryMap erstellen </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pämien aktivieren/deaktivieren </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Prämien löschen </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Prämien bearbeiten </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Userstorymap update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+    <t>Iteraton 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Besitzer/Besucher CRUD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Marlett"/>
+        <charset val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -609,188 +909,95 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Prämien filtern (Usermanagement) x</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Locations anzeigen AndroidApp </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Locations-Details anzeigen AndroidApp </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Locations filtern AndroidApp </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Location Routenplaner AndroidApp </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Usermanagement mit Firebase </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Login für Webapp mit Firebase </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Registrieren für Webapp mit Firebase </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Marlett"/>
-        <charset val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Besitzer/Besucher CRUD
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Boni-System</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> x</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 5 bis </t>
+  </si>
+  <si>
+    <t>Sprint 6 bis ?</t>
+  </si>
+  <si>
+    <t>WebApp Bug fixing
+WebApp um Sicherheits-Module ergänzen
+WebApp Loading-Animations hinzufügen
+Profil updaten WebApp</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prämien anzeigen AndroidApp
 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t>Boni-System</t>
     </r>
-  </si>
-  <si>
-    <t>Rezensionen anzeigen WebApp
-Rezensionen updaten WebApp
-Rezensionen erstellen WebApp
-Rezensionen löschen WebApp
-Rezensionen anzeigen AndroidApp</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Prämien filtern (Usermanagement)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Boni-System</t>
-    </r>
-  </si>
-  <si>
-    <t>der Usertories lösen, kümmert sich Sonnek um das Backend bzw Datenbankverbindung jeder Userstory</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Boni-System AndroidApp
+Boni-System Bonusverlauf anzeigen AndroidApp
+Boni-System Bonusverlauf anzeigen WebApp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Boni-Sytem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Boni-Sytem CRUD
+Login AndroidApp
+Registrieren AndroidApp
+Profil updaten AndroidApp
+Rezensionen anzeigen AndroidApp
+Rezensionen updaten AndroidApp
+Rezensionen löschen AndroidApp
+Rezensionen erstellen AndroidApp</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -861,7 +1068,17 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Marlett"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -904,7 +1121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -964,28 +1181,34 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1212,8 +1435,8 @@
   </sheetPr>
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1222,55 +1445,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="33"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1283,8 +1506,8 @@
       </c>
       <c r="C7" s="3"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -1301,10 +1524,10 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1324,42 +1547,42 @@
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="36"/>
+      <c r="A13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="35"/>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
     </row>
     <row r="15" spans="1:10" s="21" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
+      <c r="A15" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="34"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1368,10 +1591,10 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1380,10 +1603,10 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1392,10 +1615,10 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
@@ -1476,10 +1699,10 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="27"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1488,10 +1711,10 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="27"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1502,10 +1725,10 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="27"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1515,10 +1738,10 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="27"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1528,10 +1751,10 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -1540,10 +1763,10 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="32"/>
+      <c r="A32" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="30"/>
       <c r="C32" s="4" t="s">
         <v>12</v>
       </c>
@@ -1552,10 +1775,10 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="34"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="4" t="s">
         <v>12</v>
       </c>
@@ -1564,10 +1787,10 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="34"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="4" t="s">
         <v>12</v>
       </c>
@@ -1576,10 +1799,10 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1588,10 +1811,10 @@
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="4" t="s">
         <v>12</v>
       </c>
@@ -1600,10 +1823,10 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="34"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="4" t="s">
         <v>12</v>
       </c>
@@ -1612,20 +1835,20 @@
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
+      <c r="A38" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="28"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1633,10 +1856,10 @@
       <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="28"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="4" t="s">
         <v>7</v>
       </c>
@@ -1644,186 +1867,186 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="28"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="36"/>
+      <c r="A42" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="30"/>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="36"/>
+      <c r="A43" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="30"/>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="28"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="28"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="28"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="28"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="28"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="28"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="28"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="28"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="28"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="27"/>
+      <c r="B53" s="33"/>
       <c r="C53" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="27"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="33"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="34"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="33"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="30"/>
+      <c r="B60" s="36"/>
       <c r="C60" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="30"/>
+      <c r="B61" s="36"/>
       <c r="C61" s="4" t="s">
         <v>40</v>
       </c>
@@ -1838,7 +2061,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -1962,7 +2185,39 @@
       <c r="C91" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="48">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A57:B57"/>
@@ -1979,41 +2234,6 @@
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2022,65 +2242,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01238BF-CC45-444D-857F-D850712E7ECB}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2101,7 +2321,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>65</v>
@@ -2123,24 +2343,24 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="11" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="23" t="s">
         <v>69</v>
       </c>
@@ -2161,21 +2381,21 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
@@ -2183,14 +2403,70 @@
         <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>82</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
update stores, components, views, errorhandling
</commit_message>
<xml_diff>
--- a/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
+++ b/SYP(MUH)/Product Backlog_Traveladvisor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Schule\Schuljahr_2019_20\SYP\Github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15664F6E-3F95-410F-AA81-639850FB43A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C11BC2-E130-4C3B-9D6C-2A64C8C8BAF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productbacklog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
   <si>
     <t>Arbeitsaufteilung:</t>
   </si>
@@ -927,9 +927,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sprint 5 bis </t>
-  </si>
-  <si>
-    <t>Sprint 6 bis ?</t>
   </si>
   <si>
     <t>WebApp Bug fixing
@@ -1121,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1181,39 +1178,45 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,17 +1448,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1464,36 +1467,36 @@
       <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1506,8 +1509,8 @@
       </c>
       <c r="C7" s="3"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -1524,10 +1527,10 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1547,10 +1550,10 @@
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1559,8 +1562,8 @@
       <c r="A14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:10" s="21" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
@@ -1570,19 +1573,19 @@
       <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1591,10 +1594,10 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1603,10 +1606,10 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1615,10 +1618,10 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
@@ -1699,10 +1702,10 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="30"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1711,10 +1714,10 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1725,10 +1728,10 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="30"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1738,10 +1741,10 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1751,10 +1754,10 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="30"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -1763,10 +1766,10 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="30"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="4" t="s">
         <v>12</v>
       </c>
@@ -1775,10 +1778,10 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="30"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="4" t="s">
         <v>12</v>
       </c>
@@ -1787,10 +1790,10 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="4" t="s">
         <v>12</v>
       </c>
@@ -1799,10 +1802,10 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="30"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1811,10 +1814,10 @@
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="29"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="4" t="s">
         <v>12</v>
       </c>
@@ -1823,10 +1826,10 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="30"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="4" t="s">
         <v>12</v>
       </c>
@@ -1845,10 +1848,10 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="34"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1856,10 +1859,10 @@
       <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="34"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="4" t="s">
         <v>7</v>
       </c>
@@ -1867,127 +1870,127 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="34"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="34"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="34"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="34"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="34"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="34"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="34"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="34"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="34"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="33"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="4" t="s">
         <v>12</v>
       </c>
@@ -1996,32 +1999,32 @@
       <c r="A55" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="31"/>
+      <c r="B56" s="34"/>
       <c r="C56" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="31"/>
+      <c r="B58" s="34"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
@@ -2030,23 +2033,23 @@
       <c r="A59" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="36"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="36"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="4" t="s">
         <v>40</v>
       </c>
@@ -2186,13 +2189,31 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="A59:C59"/>
@@ -2208,32 +2229,14 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2244,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01238BF-CC45-444D-857F-D850712E7ECB}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2256,38 +2259,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
@@ -2297,10 +2300,10 @@
       <c r="C5" s="32"/>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2357,10 +2360,10 @@
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="39"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="23" t="s">
         <v>69</v>
       </c>
@@ -2417,56 +2420,55 @@
       <c r="C17" s="32"/>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="27" t="s">
-        <v>88</v>
-      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C19" s="40"/>
+    </row>
+    <row r="20" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:3" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="26"/>
+      <c r="B22" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:C1"/>
@@ -2475,6 +2477,7 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>